<commit_message>
First Difference done, Early Stop, Refactoring
</commit_message>
<xml_diff>
--- a/Performance Notes/win performance.xlsx
+++ b/Performance Notes/win performance.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Uni Goethe\Informatik\BA\Präsis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Uni Goethe\Informatik\BA\Python_Wide_Field_Deconvolution\Performance Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7816CED-D3FC-4F20-9DC0-BF7FE57B3DA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49513C73-78B6-42A1-BE21-FBFD537CC30F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Single Main Thread" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
-    <sheet name="Forcing 100% Multiprocessing" sheetId="2" r:id="rId3"/>
+    <sheet name="Forcing 100% Multiprocessing" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -135,7 +135,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -196,7 +196,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -701,136 +701,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E80F79B-15B9-4A06-A683-7ECED69F271A}">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="9">
-        <v>4</v>
-      </c>
-      <c r="C2" s="8">
-        <v>64</v>
-      </c>
-      <c r="D2" s="8">
-        <v>16</v>
-      </c>
-      <c r="E2">
-        <f>C2*D2/100</f>
-        <v>10.24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="9">
-        <v>6.5</v>
-      </c>
-      <c r="C3" s="8">
-        <v>52</v>
-      </c>
-      <c r="D3" s="8">
-        <v>22</v>
-      </c>
-      <c r="E3" s="8">
-        <f>C3*D3/100</f>
-        <v>11.44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="9">
-        <v>12</v>
-      </c>
-      <c r="C4" s="8">
-        <v>48</v>
-      </c>
-      <c r="D4" s="8">
-        <v>36</v>
-      </c>
-      <c r="E4" s="8">
-        <f>C4*D4/100</f>
-        <v>17.28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="9">
-        <v>26</v>
-      </c>
-      <c r="C5" s="8">
-        <v>52</v>
-      </c>
-      <c r="D5" s="8">
-        <v>40</v>
-      </c>
-      <c r="E5" s="8">
-        <f>C5*D5/100</f>
-        <v>20.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="9">
-        <v>85</v>
-      </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="9">
-        <v>75</v>
-      </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A952A5-21B9-48A5-8083-5841DF33B9DD}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
@@ -882,4 +756,130 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E80F79B-15B9-4A06-A683-7ECED69F271A}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="9">
+        <v>4</v>
+      </c>
+      <c r="C2" s="8">
+        <v>64</v>
+      </c>
+      <c r="D2" s="8">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <f>C2*D2/100</f>
+        <v>10.24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="9">
+        <v>6.5</v>
+      </c>
+      <c r="C3" s="8">
+        <v>52</v>
+      </c>
+      <c r="D3" s="8">
+        <v>22</v>
+      </c>
+      <c r="E3" s="8">
+        <f>C3*D3/100</f>
+        <v>11.44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="9">
+        <v>12</v>
+      </c>
+      <c r="C4" s="8">
+        <v>48</v>
+      </c>
+      <c r="D4" s="8">
+        <v>36</v>
+      </c>
+      <c r="E4" s="8">
+        <f>C4*D4/100</f>
+        <v>17.28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="9">
+        <v>26</v>
+      </c>
+      <c r="C5" s="8">
+        <v>52</v>
+      </c>
+      <c r="D5" s="8">
+        <v>40</v>
+      </c>
+      <c r="E5" s="8">
+        <f>C5*D5/100</f>
+        <v>20.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="9">
+        <v>85</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="9">
+        <v>75</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Big Commit before refactoring to Module
</commit_message>
<xml_diff>
--- a/Performance Notes/win performance.xlsx
+++ b/Performance Notes/win performance.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Uni Goethe\Informatik\BA\Python_Wide_Field_Deconvolution\Performance Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49513C73-78B6-42A1-BE21-FBFD537CC30F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915C3D2D-9B66-4512-A58E-C7576A4898CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Single Main Thread" sheetId="1" r:id="rId1"/>
     <sheet name="Forcing 100% Multiprocessing" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Rand Perf scaling T" sheetId="3" r:id="rId3"/>
+    <sheet name="JonasPerfScalingT" sheetId="4" r:id="rId4"/>
+    <sheet name="JonasPerfScalingP" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
   <si>
     <t>Algo</t>
   </si>
@@ -128,6 +130,60 @@
   </si>
   <si>
     <t>Mit MP</t>
+  </si>
+  <si>
+    <t>Dimension</t>
+  </si>
+  <si>
+    <t>Convar Time</t>
+  </si>
+  <si>
+    <t>25x10000</t>
+  </si>
+  <si>
+    <t>50x10000</t>
+  </si>
+  <si>
+    <t>100x10000</t>
+  </si>
+  <si>
+    <t>200x10000</t>
+  </si>
+  <si>
+    <t>400x10000</t>
+  </si>
+  <si>
+    <t>Early Stopped at x Iters</t>
+  </si>
+  <si>
+    <t>10k Iter Time (estimated)</t>
+  </si>
+  <si>
+    <t>10k Iter Time (real run)</t>
+  </si>
+  <si>
+    <t>CPU% (real run)</t>
+  </si>
+  <si>
+    <t>Mid Convar immer ~0,15s</t>
+  </si>
+  <si>
+    <t>Alle Angaben in Sekunden</t>
+  </si>
+  <si>
+    <t>400x5000</t>
+  </si>
+  <si>
+    <t>400x2500</t>
+  </si>
+  <si>
+    <t>400x1250</t>
+  </si>
+  <si>
+    <t>400x625</t>
+  </si>
+  <si>
+    <t>Als Algorithmus Convar_np</t>
   </si>
 </sst>
 </file>
@@ -174,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -197,6 +253,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,9 +762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92A952A5-21B9-48A5-8083-5841DF33B9DD}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -763,10 +819,13 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F5"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
@@ -882,4 +941,291 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD31A5C-A301-4651-8807-A5F281E61AC5}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2">
+        <v>31.92</v>
+      </c>
+      <c r="C2" s="10">
+        <v>6098</v>
+      </c>
+      <c r="D2" s="10">
+        <f>B2*(1/(C2/10000))</f>
+        <v>52.345031157756644</v>
+      </c>
+      <c r="E2" s="11">
+        <v>43</v>
+      </c>
+      <c r="F2">
+        <v>51.73</v>
+      </c>
+      <c r="G2" s="11">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="10">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="C3" s="10">
+        <v>412</v>
+      </c>
+      <c r="D3" s="10">
+        <f>B3*(1/(C3/10000))</f>
+        <v>115.77669902912619</v>
+      </c>
+      <c r="E3" s="11">
+        <v>42</v>
+      </c>
+      <c r="F3" s="10">
+        <v>110.14</v>
+      </c>
+      <c r="G3" s="11">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="10">
+        <v>5.76</v>
+      </c>
+      <c r="C4" s="10">
+        <v>232</v>
+      </c>
+      <c r="D4" s="10">
+        <f>B4*(1/(C4/10000))</f>
+        <v>248.27586206896552</v>
+      </c>
+      <c r="E4" s="11">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="10">
+        <v>12.03</v>
+      </c>
+      <c r="C5" s="10">
+        <v>234</v>
+      </c>
+      <c r="D5" s="10">
+        <f>B5*(1/(C5/10000))</f>
+        <v>514.10256410256409</v>
+      </c>
+      <c r="E5" s="11">
+        <v>52</v>
+      </c>
+      <c r="F5" s="10">
+        <v>496.8</v>
+      </c>
+      <c r="G5" s="11">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="10">
+        <v>24.08</v>
+      </c>
+      <c r="C6" s="10">
+        <v>232</v>
+      </c>
+      <c r="D6" s="10">
+        <f>B6*(1/(C6/10000))</f>
+        <v>1037.9310344827586</v>
+      </c>
+      <c r="E6" s="11">
+        <v>58</v>
+      </c>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D292344-3CE0-47E7-8CFA-CFFE67F807FB}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I7" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I8" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I9" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Pre Intelligence Adaptive LR
</commit_message>
<xml_diff>
--- a/Performance Notes/win performance.xlsx
+++ b/Performance Notes/win performance.xlsx
@@ -5,19 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Uni Goethe\Informatik\BA\Python_Wide_Field_Deconvolution\Performance Notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Uni Goethe\Informatik\BA\PyWFDeconv\Performance Notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915C3D2D-9B66-4512-A58E-C7576A4898CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9097F223-CFE8-4DBF-83E0-4ABF2A9F3408}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="774" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Single Main Thread" sheetId="1" r:id="rId1"/>
     <sheet name="Forcing 100% Multiprocessing" sheetId="2" r:id="rId2"/>
     <sheet name="Rand Perf scaling T" sheetId="3" r:id="rId3"/>
-    <sheet name="JonasPerfScalingT" sheetId="4" r:id="rId4"/>
-    <sheet name="JonasPerfScalingP" sheetId="5" r:id="rId5"/>
+    <sheet name="JonasPerfScalingT10000" sheetId="4" r:id="rId4"/>
+    <sheet name="JonasPerfScalingT5000" sheetId="6" r:id="rId5"/>
+    <sheet name="JonasPerfScalingT500" sheetId="9" r:id="rId6"/>
+    <sheet name="JonasPerfScalingT100" sheetId="7" r:id="rId7"/>
+    <sheet name="JonasPerfScalingP" sheetId="5" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
   <si>
     <t>Algo</t>
   </si>
@@ -184,6 +187,48 @@
   </si>
   <si>
     <t>Als Algorithmus Convar_np</t>
+  </si>
+  <si>
+    <t>25x5000</t>
+  </si>
+  <si>
+    <t>50x5000</t>
+  </si>
+  <si>
+    <t>100x5000</t>
+  </si>
+  <si>
+    <t>200x5000</t>
+  </si>
+  <si>
+    <t>400x100</t>
+  </si>
+  <si>
+    <t>200x100</t>
+  </si>
+  <si>
+    <t>100x100</t>
+  </si>
+  <si>
+    <t>50x100</t>
+  </si>
+  <si>
+    <t>25x100</t>
+  </si>
+  <si>
+    <t>400x500</t>
+  </si>
+  <si>
+    <t>200x500</t>
+  </si>
+  <si>
+    <t>100x500</t>
+  </si>
+  <si>
+    <t>50x500</t>
+  </si>
+  <si>
+    <t>25x500</t>
   </si>
 </sst>
 </file>
@@ -818,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E80F79B-15B9-4A06-A683-7ECED69F271A}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,8 +992,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD31A5C-A301-4651-8807-A5F281E61AC5}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,10 +1161,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D292344-3CE0-47E7-8CFA-CFFE67F807FB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF846A4-DA3B-4D0D-8EA6-8BF20764B1DD}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1154,14 +1201,432 @@
       <c r="G1" s="8" t="s">
         <v>41</v>
       </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="8">
+        <v>9.1</v>
+      </c>
+      <c r="C2" s="10">
+        <v>6842</v>
+      </c>
+      <c r="D2" s="10">
+        <f>B2*(1/(C2/10000))</f>
+        <v>13.300204618532591</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="10">
+        <v>2.29</v>
+      </c>
+      <c r="C3" s="10">
+        <v>390</v>
+      </c>
+      <c r="D3" s="10">
+        <f>B3*(1/(C3/10000))</f>
+        <v>58.717948717948723</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="10">
+        <v>2.84</v>
+      </c>
+      <c r="C4" s="10">
+        <v>228</v>
+      </c>
+      <c r="D4" s="10">
+        <f>B4*(1/(C4/10000))</f>
+        <v>124.56140350877192</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="10">
+        <v>6.06</v>
+      </c>
+      <c r="C5" s="10">
+        <v>233</v>
+      </c>
+      <c r="D5" s="10">
+        <f>B5*(1/(C5/10000))</f>
+        <v>260.0858369098712</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="10">
+        <v>13.25</v>
+      </c>
+      <c r="C6" s="10">
+        <v>231</v>
+      </c>
+      <c r="D6" s="10">
+        <f>B6*(1/(C6/10000))</f>
+        <v>573.59307359307365</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8524B57D-D2A6-458E-8BE2-C254FB98542F}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="8">
+        <v>3.31</v>
+      </c>
+      <c r="C2" s="11">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="10">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="C3" s="11">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="8">
+        <v>7.34</v>
+      </c>
+      <c r="C4" s="8">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="10">
+        <v>16.03</v>
+      </c>
+      <c r="C5" s="11">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="8">
+        <v>56.18</v>
+      </c>
+      <c r="C6" s="11">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60750254-1BB7-4DAA-96B3-D26DF10DF572}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="8">
+        <v>0.32</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="10">
+        <v>0.67</v>
+      </c>
+      <c r="C3" s="11"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3.61</v>
+      </c>
+      <c r="C4" s="8">
+        <v>58</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="10">
+        <v>6.25</v>
+      </c>
+      <c r="C5" s="11">
+        <v>70</v>
+      </c>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="8">
+        <v>13.96</v>
+      </c>
+      <c r="C6" s="11">
+        <v>86</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D292344-3CE0-47E7-8CFA-CFFE67F807FB}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
+      <c r="B2" s="8">
+        <v>1.89</v>
+      </c>
+      <c r="C2" s="10">
+        <v>231</v>
+      </c>
+      <c r="D2" s="10">
+        <f t="shared" ref="D2:D5" si="0">B2*(1/(C2/10000))</f>
+        <v>81.818181818181813</v>
+      </c>
       <c r="E2" s="11"/>
       <c r="F2" s="8"/>
       <c r="G2" s="11"/>
@@ -1170,9 +1635,16 @@
       <c r="A3" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
+      <c r="B3" s="10">
+        <v>3.82</v>
+      </c>
+      <c r="C3" s="10">
+        <v>230</v>
+      </c>
+      <c r="D3" s="10">
+        <f t="shared" si="0"/>
+        <v>166.08695652173913</v>
+      </c>
       <c r="E3" s="11"/>
       <c r="F3" s="10"/>
       <c r="G3" s="11"/>
@@ -1181,9 +1653,16 @@
       <c r="A4" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
+      <c r="B4" s="10">
+        <v>7.28</v>
+      </c>
+      <c r="C4" s="10">
+        <v>229</v>
+      </c>
+      <c r="D4" s="10">
+        <f t="shared" si="0"/>
+        <v>317.90393013100436</v>
+      </c>
       <c r="E4" s="11"/>
       <c r="F4" s="8"/>
       <c r="G4" s="11"/>
@@ -1192,9 +1671,16 @@
       <c r="A5" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
+      <c r="B5" s="10">
+        <v>13.91</v>
+      </c>
+      <c r="C5" s="10">
+        <v>231</v>
+      </c>
+      <c r="D5" s="10">
+        <f t="shared" si="0"/>
+        <v>602.16450216450221</v>
+      </c>
       <c r="E5" s="11"/>
       <c r="F5" s="8"/>
       <c r="G5" s="11"/>
@@ -1203,9 +1689,16 @@
       <c r="A6" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
+      <c r="B6" s="10">
+        <v>25.68</v>
+      </c>
+      <c r="C6" s="10">
+        <v>232</v>
+      </c>
+      <c r="D6" s="10">
+        <f>B6*(1/(C6/10000))</f>
+        <v>1106.8965517241379</v>
+      </c>
       <c r="E6" s="11"/>
       <c r="F6" s="8"/>
       <c r="G6" s="11"/>

</xml_diff>